<commit_message>
update data source excel
</commit_message>
<xml_diff>
--- a/src/main/resources/datasource.xlsx
+++ b/src/main/resources/datasource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijayan.s01\Desktop\Java WorkSpace\E2EAPITesting\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF256AE5-C247-4324-A6C1-18EDB3570E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0521AAD0-9E69-4A7D-AB9B-C953F5B75B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,15 +450,15 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">"testuser" &amp; RANDBETWEEN(1,99999)</f>
-        <v>testuser24634</v>
+        <v>testuser40332</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">"password"&amp;RANDBETWEEN(10, 10000)</f>
-        <v>password5182</v>
+        <v>password123</v>
       </c>
       <c r="D2" t="str">
         <f ca="1">_xlfn.CONCAT(B2,"@yahoo.com")</f>
-        <v>testuser24634@yahoo.com</v>
+        <v>testuser40332@yahoo.com</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -468,7 +468,7 @@
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(6999999999,9999999999)</f>
-        <v>7249146188</v>
+        <v>8765586832</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -477,15 +477,15 @@
       </c>
       <c r="B3" t="str">
         <f ca="1">B2</f>
-        <v>testuser24634</v>
+        <v>testuser40332</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="0">"password"&amp;RANDBETWEEN(10, 10000)</f>
-        <v>password204</v>
+        <v>password310</v>
       </c>
       <c r="D3" t="str">
         <f ca="1">_xlfn.CONCAT("uniqueuser" &amp; RANDBETWEEN(1,99999),"@yahoo.com")</f>
-        <v>uniqueuser14401@yahoo.com</v>
+        <v>uniqueuser70462@yahoo.com</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -495,7 +495,7 @@
       </c>
       <c r="G3">
         <f ca="1">RANDBETWEEN(6999999999,9999999999)</f>
-        <v>7013829805</v>
+        <v>7327638220</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -504,15 +504,15 @@
       </c>
       <c r="B4" t="str">
         <f ca="1">"testuser" &amp; RANDBETWEEN(1,99999)</f>
-        <v>testuser14461</v>
+        <v>testuser45144</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>password1756</v>
+        <v>password2638</v>
       </c>
       <c r="D4" t="str">
         <f ca="1">D2</f>
-        <v>testuser24634@yahoo.com</v>
+        <v>testuser40332@yahoo.com</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -522,7 +522,7 @@
       </c>
       <c r="G4">
         <f ca="1">RANDBETWEEN(6999999999,9999999999)</f>
-        <v>9036953826</v>
+        <v>7718189184</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -531,14 +531,14 @@
       </c>
       <c r="B5" t="str">
         <f ca="1">"testuser" &amp; RANDBETWEEN(1,99999)</f>
-        <v>testuser67116</v>
+        <v>testuser82728</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="str">
         <f ca="1">_xlfn.CONCAT(B5,"@yahoo.com")</f>
-        <v>testuser67116@yahoo.com</v>
+        <v>testuser82728@yahoo.com</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="G5">
         <f ca="1">RANDBETWEEN(6999999999,9999999999)</f>
-        <v>7682708759</v>
+        <v>9962458859</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -557,11 +557,11 @@
       </c>
       <c r="B6" t="str">
         <f ca="1">"testuser" &amp; RANDBETWEEN(1,99999)</f>
-        <v>testuser1770</v>
+        <v>testuser58229</v>
       </c>
       <c r="D6" t="str">
         <f ca="1">_xlfn.CONCAT(B6,"@yahoo.com")</f>
-        <v>testuser1770@yahoo.com</v>
+        <v>testuser58229@yahoo.com</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -571,7 +571,7 @@
       </c>
       <c r="G6">
         <f ca="1">RANDBETWEEN(6999999999,9999999999)</f>
-        <v>7598823955</v>
+        <v>8295687443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>